<commit_message>
descriçao do que voce fez
</commit_message>
<xml_diff>
--- a/planilhaderotascc19.xlsx
+++ b/planilhaderotascc19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Robo-Baixa-Entregas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_A83E597D702693C2E552E180EFAE55EF9C0ADDBF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3159D2E9-D0C4-4925-A23B-40A64206405C}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_A83E597D702693C2E552E180EFAE55EF9C0ADDBF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D829E117-D418-4616-88F7-B1B9CDCBCE2B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5606" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5726" uniqueCount="518">
   <si>
     <t>Data</t>
   </si>
@@ -1567,6 +1567,30 @@
   <si>
     <t>MZB CHOCOLATES LTDA</t>
   </si>
+  <si>
+    <t>47.735.028/0001-30</t>
+  </si>
+  <si>
+    <t>GB CHOCOLATES LTDA</t>
+  </si>
+  <si>
+    <t>51.560.917/0001-81</t>
+  </si>
+  <si>
+    <t>MB CHOCOLATES LTDA</t>
+  </si>
+  <si>
+    <t>05.287.975/0001-66</t>
+  </si>
+  <si>
+    <t>MARCIA REGINA ZAMBON BARALDI CHOCOL</t>
+  </si>
+  <si>
+    <t>10.345.781/0001-00</t>
+  </si>
+  <si>
+    <t>MARIA EDUARDA BARALDI - EPP</t>
+  </si>
 </sst>
 </file>
 
@@ -1735,9 +1759,9 @@
     <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2748,10 +2772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T1072"/>
+  <dimension ref="A1:T1092"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1065" workbookViewId="0">
-      <selection activeCell="A1073" sqref="A1073"/>
+    <sheetView tabSelected="1" topLeftCell="A1085" workbookViewId="0">
+      <selection activeCell="A1093" sqref="A1093"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -49692,914 +49716,1874 @@
       <c r="R1052" s="19"/>
     </row>
     <row r="1053" spans="1:18">
-      <c r="A1053" s="26">
-        <v>45447</v>
-      </c>
-      <c r="B1053" s="25" t="s">
+      <c r="A1053" s="20">
+        <v>45447</v>
+      </c>
+      <c r="B1053" s="19" t="s">
         <v>326</v>
       </c>
-      <c r="C1053" s="25" t="s">
+      <c r="C1053" s="19" t="s">
         <v>484</v>
       </c>
-      <c r="D1053" s="25">
+      <c r="D1053" s="19">
         <v>197570</v>
       </c>
-      <c r="E1053" s="25">
-        <v>2</v>
-      </c>
-      <c r="F1053" s="27">
+      <c r="E1053" s="19">
+        <v>2</v>
+      </c>
+      <c r="F1053" s="21">
         <v>1469576</v>
       </c>
-      <c r="G1053" s="25" t="s">
+      <c r="G1053" s="19" t="s">
         <v>485</v>
       </c>
-      <c r="H1053" s="25" t="s">
+      <c r="H1053" s="19" t="s">
         <v>481</v>
       </c>
-      <c r="I1053" s="28">
+      <c r="I1053" s="22">
         <v>1605389</v>
       </c>
-      <c r="J1053" s="25">
+      <c r="J1053" s="19">
         <v>1</v>
       </c>
-      <c r="K1053" s="25">
+      <c r="K1053" s="19">
         <v>3.51</v>
       </c>
-      <c r="L1053" s="25">
+      <c r="L1053" s="19">
         <v>200.27</v>
       </c>
-      <c r="M1053" s="25"/>
-      <c r="N1053" s="25"/>
-      <c r="O1053" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1053" s="25"/>
-      <c r="Q1053" s="25"/>
-      <c r="R1053" s="25"/>
+      <c r="M1053" s="19"/>
+      <c r="N1053" s="19"/>
+      <c r="O1053" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1053" s="19"/>
+      <c r="Q1053" s="19"/>
+      <c r="R1053" s="19"/>
     </row>
     <row r="1054" spans="1:18">
-      <c r="A1054" s="26">
-        <v>45447</v>
-      </c>
-      <c r="B1054" s="25" t="s">
+      <c r="A1054" s="20">
+        <v>45447</v>
+      </c>
+      <c r="B1054" s="19" t="s">
         <v>326</v>
       </c>
-      <c r="C1054" s="25" t="s">
+      <c r="C1054" s="19" t="s">
         <v>484</v>
       </c>
-      <c r="D1054" s="25">
+      <c r="D1054" s="19">
         <v>197570</v>
       </c>
-      <c r="E1054" s="25">
-        <v>2</v>
-      </c>
-      <c r="F1054" s="27">
+      <c r="E1054" s="19">
+        <v>2</v>
+      </c>
+      <c r="F1054" s="21">
         <v>1469577</v>
       </c>
-      <c r="G1054" s="25" t="s">
+      <c r="G1054" s="19" t="s">
         <v>485</v>
       </c>
-      <c r="H1054" s="25" t="s">
+      <c r="H1054" s="19" t="s">
         <v>481</v>
       </c>
-      <c r="I1054" s="28">
+      <c r="I1054" s="22">
         <v>1605389</v>
       </c>
-      <c r="J1054" s="25">
+      <c r="J1054" s="19">
         <v>1</v>
       </c>
-      <c r="K1054" s="25">
+      <c r="K1054" s="19">
         <v>2.25</v>
       </c>
-      <c r="L1054" s="25">
+      <c r="L1054" s="19">
         <v>208.31</v>
       </c>
-      <c r="M1054" s="25"/>
-      <c r="N1054" s="25"/>
-      <c r="O1054" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1054" s="25"/>
-      <c r="Q1054" s="25"/>
-      <c r="R1054" s="25"/>
+      <c r="M1054" s="19"/>
+      <c r="N1054" s="19"/>
+      <c r="O1054" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1054" s="19"/>
+      <c r="Q1054" s="19"/>
+      <c r="R1054" s="19"/>
     </row>
     <row r="1055" spans="1:18">
-      <c r="A1055" s="26">
-        <v>45447</v>
-      </c>
-      <c r="B1055" s="25" t="s">
+      <c r="A1055" s="20">
+        <v>45447</v>
+      </c>
+      <c r="B1055" s="19" t="s">
         <v>326</v>
       </c>
-      <c r="C1055" s="25" t="s">
+      <c r="C1055" s="19" t="s">
         <v>486</v>
       </c>
-      <c r="D1055" s="25">
+      <c r="D1055" s="19">
         <v>197570</v>
       </c>
-      <c r="E1055" s="25">
-        <v>2</v>
-      </c>
-      <c r="F1055" s="27">
+      <c r="E1055" s="19">
+        <v>2</v>
+      </c>
+      <c r="F1055" s="21">
         <v>1469582</v>
       </c>
-      <c r="G1055" s="25" t="s">
+      <c r="G1055" s="19" t="s">
         <v>487</v>
       </c>
-      <c r="H1055" s="25" t="s">
+      <c r="H1055" s="19" t="s">
         <v>481</v>
       </c>
-      <c r="I1055" s="28">
+      <c r="I1055" s="22">
         <v>1605413</v>
       </c>
-      <c r="J1055" s="25">
+      <c r="J1055" s="19">
         <v>3</v>
       </c>
-      <c r="K1055" s="25">
+      <c r="K1055" s="19">
         <v>8.98</v>
       </c>
-      <c r="L1055" s="25">
+      <c r="L1055" s="19">
         <v>384.95</v>
       </c>
-      <c r="M1055" s="25"/>
-      <c r="N1055" s="25"/>
-      <c r="O1055" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1055" s="25"/>
-      <c r="Q1055" s="25"/>
-      <c r="R1055" s="25"/>
+      <c r="M1055" s="19"/>
+      <c r="N1055" s="19"/>
+      <c r="O1055" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1055" s="19"/>
+      <c r="Q1055" s="19"/>
+      <c r="R1055" s="19"/>
     </row>
     <row r="1056" spans="1:18">
-      <c r="A1056" s="26">
-        <v>45447</v>
-      </c>
-      <c r="B1056" s="25">
+      <c r="A1056" s="20">
+        <v>45447</v>
+      </c>
+      <c r="B1056" s="19">
         <v>77</v>
       </c>
-      <c r="C1056" s="25">
+      <c r="C1056" s="19">
         <v>782.01</v>
       </c>
-      <c r="D1056" s="30">
+      <c r="D1056" s="24">
         <v>46559.01</v>
       </c>
-      <c r="E1056" s="25"/>
-      <c r="F1056" s="25"/>
-      <c r="G1056" s="25"/>
-      <c r="H1056" s="25"/>
-      <c r="I1056" s="25"/>
-      <c r="J1056" s="25"/>
-      <c r="K1056" s="25"/>
-      <c r="L1056" s="25"/>
-      <c r="M1056" s="25"/>
-      <c r="N1056" s="25"/>
-      <c r="O1056" s="25"/>
-      <c r="P1056" s="25"/>
-      <c r="Q1056" s="25"/>
-      <c r="R1056" s="25"/>
+      <c r="E1056" s="19"/>
+      <c r="F1056" s="19"/>
+      <c r="G1056" s="19"/>
+      <c r="H1056" s="19"/>
+      <c r="I1056" s="19"/>
+      <c r="J1056" s="19"/>
+      <c r="K1056" s="19"/>
+      <c r="L1056" s="19"/>
+      <c r="M1056" s="19"/>
+      <c r="N1056" s="19"/>
+      <c r="O1056" s="19"/>
+      <c r="P1056" s="19"/>
+      <c r="Q1056" s="19"/>
+      <c r="R1056" s="19"/>
     </row>
     <row r="1057" spans="1:18">
-      <c r="A1057" s="26">
-        <v>45447</v>
-      </c>
-      <c r="B1057" s="25" t="s">
+      <c r="A1057" s="20">
+        <v>45447</v>
+      </c>
+      <c r="B1057" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="C1057" s="25" t="s">
+      <c r="C1057" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="D1057" s="25" t="s">
+      <c r="D1057" s="19" t="s">
         <v>499</v>
       </c>
-      <c r="E1057" s="25"/>
-      <c r="F1057" s="25"/>
-      <c r="G1057" s="25"/>
-      <c r="H1057" s="25"/>
-      <c r="I1057" s="25"/>
-      <c r="J1057" s="25"/>
-      <c r="K1057" s="25"/>
-      <c r="L1057" s="25"/>
-      <c r="M1057" s="25"/>
-      <c r="N1057" s="25"/>
-      <c r="O1057" s="25"/>
-      <c r="P1057" s="25"/>
-      <c r="Q1057" s="25"/>
-      <c r="R1057" s="25"/>
+      <c r="E1057" s="19"/>
+      <c r="F1057" s="19"/>
+      <c r="G1057" s="19"/>
+      <c r="H1057" s="19"/>
+      <c r="I1057" s="19"/>
+      <c r="J1057" s="19"/>
+      <c r="K1057" s="19"/>
+      <c r="L1057" s="19"/>
+      <c r="M1057" s="19"/>
+      <c r="N1057" s="19"/>
+      <c r="O1057" s="19"/>
+      <c r="P1057" s="19"/>
+      <c r="Q1057" s="19"/>
+      <c r="R1057" s="19"/>
     </row>
     <row r="1058" spans="1:18">
-      <c r="A1058" s="26">
-        <v>45447</v>
-      </c>
-      <c r="B1058" s="25" t="s">
+      <c r="A1058" s="20">
+        <v>45447</v>
+      </c>
+      <c r="B1058" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1058" s="25" t="s">
+      <c r="C1058" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="D1058" s="25" t="s">
+      <c r="D1058" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E1058" s="25" t="s">
+      <c r="E1058" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F1058" s="25" t="s">
+      <c r="F1058" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="G1058" s="25" t="s">
+      <c r="G1058" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="H1058" s="25" t="s">
+      <c r="H1058" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="I1058" s="25" t="s">
+      <c r="I1058" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J1058" s="25" t="s">
+      <c r="J1058" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="K1058" s="25" t="s">
+      <c r="K1058" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="L1058" s="25" t="s">
+      <c r="L1058" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="M1058" s="25"/>
-      <c r="N1058" s="25"/>
-      <c r="O1058" s="25"/>
-      <c r="P1058" s="25"/>
-      <c r="Q1058" s="25"/>
-      <c r="R1058" s="25"/>
+      <c r="M1058" s="19"/>
+      <c r="N1058" s="19"/>
+      <c r="O1058" s="19"/>
+      <c r="P1058" s="19"/>
+      <c r="Q1058" s="19"/>
+      <c r="R1058" s="19"/>
     </row>
     <row r="1059" spans="1:18">
-      <c r="A1059" s="26">
-        <v>45447</v>
-      </c>
-      <c r="B1059" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1059" s="25" t="s">
+      <c r="A1059" s="20">
+        <v>45447</v>
+      </c>
+      <c r="B1059" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1059" s="19" t="s">
         <v>500</v>
       </c>
-      <c r="D1059" s="25">
-        <v>197402</v>
-      </c>
-      <c r="E1059" s="25">
-        <v>2</v>
-      </c>
-      <c r="F1059" s="27">
+      <c r="D1059" s="19">
+        <v>197402</v>
+      </c>
+      <c r="E1059" s="19">
+        <v>2</v>
+      </c>
+      <c r="F1059" s="21">
         <v>1460456</v>
       </c>
-      <c r="G1059" s="25" t="s">
+      <c r="G1059" s="19" t="s">
         <v>501</v>
       </c>
-      <c r="H1059" s="25" t="s">
+      <c r="H1059" s="19" t="s">
         <v>502</v>
       </c>
-      <c r="I1059" s="28">
+      <c r="I1059" s="22">
         <v>1603758</v>
       </c>
-      <c r="J1059" s="25">
+      <c r="J1059" s="19">
         <v>16</v>
       </c>
-      <c r="K1059" s="25">
+      <c r="K1059" s="19">
         <v>23.02</v>
       </c>
-      <c r="L1059" s="30">
+      <c r="L1059" s="24">
         <v>1016.83</v>
       </c>
-      <c r="M1059" s="25" t="s">
+      <c r="M1059" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="N1059" s="31"/>
-      <c r="O1059" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1059" s="25"/>
-      <c r="Q1059" s="25"/>
-      <c r="R1059" s="25"/>
+      <c r="N1059" s="19"/>
+      <c r="O1059" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1059" s="19"/>
+      <c r="Q1059" s="19"/>
+      <c r="R1059" s="19"/>
     </row>
     <row r="1060" spans="1:18">
-      <c r="A1060" s="26">
-        <v>45447</v>
-      </c>
-      <c r="B1060" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1060" s="25" t="s">
+      <c r="A1060" s="20">
+        <v>45447</v>
+      </c>
+      <c r="B1060" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1060" s="19" t="s">
         <v>500</v>
       </c>
-      <c r="D1060" s="25">
-        <v>197402</v>
-      </c>
-      <c r="E1060" s="25">
-        <v>2</v>
-      </c>
-      <c r="F1060" s="27">
+      <c r="D1060" s="19">
+        <v>197402</v>
+      </c>
+      <c r="E1060" s="19">
+        <v>2</v>
+      </c>
+      <c r="F1060" s="21">
         <v>1460457</v>
       </c>
-      <c r="G1060" s="25" t="s">
+      <c r="G1060" s="19" t="s">
         <v>501</v>
       </c>
-      <c r="H1060" s="25" t="s">
+      <c r="H1060" s="19" t="s">
         <v>502</v>
       </c>
-      <c r="I1060" s="28">
+      <c r="I1060" s="22">
         <v>1603758</v>
       </c>
-      <c r="J1060" s="25">
+      <c r="J1060" s="19">
         <v>4</v>
       </c>
-      <c r="K1060" s="25">
+      <c r="K1060" s="19">
         <v>17.920000000000002</v>
       </c>
-      <c r="L1060" s="30">
+      <c r="L1060" s="24">
         <v>1251.72</v>
       </c>
-      <c r="M1060" s="25" t="s">
+      <c r="M1060" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="N1060" s="31"/>
-      <c r="O1060" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1060" s="25"/>
-      <c r="Q1060" s="25"/>
-      <c r="R1060" s="25"/>
+      <c r="N1060" s="19"/>
+      <c r="O1060" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1060" s="19"/>
+      <c r="Q1060" s="19"/>
+      <c r="R1060" s="19"/>
     </row>
     <row r="1061" spans="1:18">
-      <c r="A1061" s="26">
-        <v>45447</v>
-      </c>
-      <c r="B1061" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1061" s="25" t="s">
+      <c r="A1061" s="20">
+        <v>45447</v>
+      </c>
+      <c r="B1061" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1061" s="19" t="s">
         <v>500</v>
       </c>
-      <c r="D1061" s="25">
-        <v>197402</v>
-      </c>
-      <c r="E1061" s="25">
-        <v>2</v>
-      </c>
-      <c r="F1061" s="27">
+      <c r="D1061" s="19">
+        <v>197402</v>
+      </c>
+      <c r="E1061" s="19">
+        <v>2</v>
+      </c>
+      <c r="F1061" s="21">
         <v>1460458</v>
       </c>
-      <c r="G1061" s="25" t="s">
+      <c r="G1061" s="19" t="s">
         <v>501</v>
       </c>
-      <c r="H1061" s="25" t="s">
+      <c r="H1061" s="19" t="s">
         <v>502</v>
       </c>
-      <c r="I1061" s="28">
+      <c r="I1061" s="22">
         <v>1603758</v>
       </c>
-      <c r="J1061" s="25">
+      <c r="J1061" s="19">
         <v>1</v>
       </c>
-      <c r="K1061" s="25">
-        <v>2</v>
-      </c>
-      <c r="L1061" s="25">
+      <c r="K1061" s="19">
+        <v>2</v>
+      </c>
+      <c r="L1061" s="19">
         <v>94.62</v>
       </c>
-      <c r="M1061" s="25" t="s">
+      <c r="M1061" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="N1061" s="31"/>
-      <c r="O1061" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1061" s="25"/>
-      <c r="Q1061" s="25"/>
-      <c r="R1061" s="25"/>
+      <c r="N1061" s="19"/>
+      <c r="O1061" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1061" s="19"/>
+      <c r="Q1061" s="19"/>
+      <c r="R1061" s="19"/>
     </row>
     <row r="1062" spans="1:18">
-      <c r="A1062" s="26">
-        <v>45447</v>
-      </c>
-      <c r="B1062" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1062" s="25" t="s">
+      <c r="A1062" s="20">
+        <v>45447</v>
+      </c>
+      <c r="B1062" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1062" s="19" t="s">
         <v>500</v>
       </c>
-      <c r="D1062" s="25">
-        <v>197402</v>
-      </c>
-      <c r="E1062" s="25">
-        <v>2</v>
-      </c>
-      <c r="F1062" s="27">
+      <c r="D1062" s="19">
+        <v>197402</v>
+      </c>
+      <c r="E1062" s="19">
+        <v>2</v>
+      </c>
+      <c r="F1062" s="21">
         <v>1460459</v>
       </c>
-      <c r="G1062" s="25" t="s">
+      <c r="G1062" s="19" t="s">
         <v>501</v>
       </c>
-      <c r="H1062" s="25" t="s">
+      <c r="H1062" s="19" t="s">
         <v>502</v>
       </c>
-      <c r="I1062" s="28">
+      <c r="I1062" s="22">
         <v>1603758</v>
       </c>
-      <c r="J1062" s="25">
+      <c r="J1062" s="19">
         <v>4</v>
       </c>
-      <c r="K1062" s="25">
+      <c r="K1062" s="19">
         <v>10.76</v>
       </c>
-      <c r="L1062" s="25">
+      <c r="L1062" s="19">
         <v>561.41</v>
       </c>
-      <c r="M1062" s="25" t="s">
+      <c r="M1062" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="N1062" s="31"/>
-      <c r="O1062" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1062" s="25"/>
-      <c r="Q1062" s="25"/>
-      <c r="R1062" s="25"/>
+      <c r="N1062" s="19"/>
+      <c r="O1062" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1062" s="19"/>
+      <c r="Q1062" s="19"/>
+      <c r="R1062" s="19"/>
     </row>
     <row r="1063" spans="1:18">
-      <c r="A1063" s="26">
-        <v>45447</v>
-      </c>
-      <c r="B1063" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1063" s="25" t="s">
+      <c r="A1063" s="20">
+        <v>45447</v>
+      </c>
+      <c r="B1063" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1063" s="19" t="s">
         <v>503</v>
       </c>
-      <c r="D1063" s="25">
-        <v>197402</v>
-      </c>
-      <c r="E1063" s="25">
-        <v>2</v>
-      </c>
-      <c r="F1063" s="27">
+      <c r="D1063" s="19">
+        <v>197402</v>
+      </c>
+      <c r="E1063" s="19">
+        <v>2</v>
+      </c>
+      <c r="F1063" s="21">
         <v>1460463</v>
       </c>
-      <c r="G1063" s="25" t="s">
+      <c r="G1063" s="19" t="s">
         <v>504</v>
       </c>
-      <c r="H1063" s="25" t="s">
+      <c r="H1063" s="19" t="s">
         <v>505</v>
       </c>
-      <c r="I1063" s="28">
+      <c r="I1063" s="22">
         <v>1603755</v>
       </c>
-      <c r="J1063" s="25">
+      <c r="J1063" s="19">
         <v>8</v>
       </c>
-      <c r="K1063" s="25">
+      <c r="K1063" s="19">
         <v>11.51</v>
       </c>
-      <c r="L1063" s="25">
+      <c r="L1063" s="19">
         <v>508.43</v>
       </c>
-      <c r="M1063" s="25" t="s">
+      <c r="M1063" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="N1063" s="31"/>
-      <c r="O1063" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1063" s="25"/>
-      <c r="Q1063" s="25"/>
-      <c r="R1063" s="25"/>
+      <c r="N1063" s="19"/>
+      <c r="O1063" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1063" s="19"/>
+      <c r="Q1063" s="19"/>
+      <c r="R1063" s="19"/>
     </row>
     <row r="1064" spans="1:18">
-      <c r="A1064" s="26">
-        <v>45447</v>
-      </c>
-      <c r="B1064" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1064" s="25" t="s">
+      <c r="A1064" s="20">
+        <v>45447</v>
+      </c>
+      <c r="B1064" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1064" s="19" t="s">
         <v>503</v>
       </c>
-      <c r="D1064" s="25">
-        <v>197402</v>
-      </c>
-      <c r="E1064" s="25">
-        <v>2</v>
-      </c>
-      <c r="F1064" s="27">
+      <c r="D1064" s="19">
+        <v>197402</v>
+      </c>
+      <c r="E1064" s="19">
+        <v>2</v>
+      </c>
+      <c r="F1064" s="21">
         <v>1460464</v>
       </c>
-      <c r="G1064" s="25" t="s">
+      <c r="G1064" s="19" t="s">
         <v>504</v>
       </c>
-      <c r="H1064" s="25" t="s">
+      <c r="H1064" s="19" t="s">
         <v>505</v>
       </c>
-      <c r="I1064" s="28">
+      <c r="I1064" s="22">
         <v>1603755</v>
       </c>
-      <c r="J1064" s="25">
+      <c r="J1064" s="19">
         <v>3</v>
       </c>
-      <c r="K1064" s="25">
+      <c r="K1064" s="19">
         <v>13.44</v>
       </c>
-      <c r="L1064" s="25">
+      <c r="L1064" s="19">
         <v>938.8</v>
       </c>
-      <c r="M1064" s="25" t="s">
+      <c r="M1064" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="N1064" s="31"/>
-      <c r="O1064" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1064" s="25"/>
-      <c r="Q1064" s="25"/>
-      <c r="R1064" s="25"/>
+      <c r="N1064" s="19"/>
+      <c r="O1064" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1064" s="19"/>
+      <c r="Q1064" s="19"/>
+      <c r="R1064" s="19"/>
     </row>
     <row r="1065" spans="1:18">
-      <c r="A1065" s="26">
-        <v>45447</v>
-      </c>
-      <c r="B1065" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1065" s="25" t="s">
+      <c r="A1065" s="20">
+        <v>45447</v>
+      </c>
+      <c r="B1065" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1065" s="19" t="s">
         <v>503</v>
       </c>
-      <c r="D1065" s="25">
-        <v>197402</v>
-      </c>
-      <c r="E1065" s="25">
-        <v>2</v>
-      </c>
-      <c r="F1065" s="27">
+      <c r="D1065" s="19">
+        <v>197402</v>
+      </c>
+      <c r="E1065" s="19">
+        <v>2</v>
+      </c>
+      <c r="F1065" s="21">
         <v>1460465</v>
       </c>
-      <c r="G1065" s="25" t="s">
+      <c r="G1065" s="19" t="s">
         <v>504</v>
       </c>
-      <c r="H1065" s="25" t="s">
+      <c r="H1065" s="19" t="s">
         <v>505</v>
       </c>
-      <c r="I1065" s="28">
+      <c r="I1065" s="22">
         <v>1603755</v>
       </c>
-      <c r="J1065" s="25">
+      <c r="J1065" s="19">
         <v>3</v>
       </c>
-      <c r="K1065" s="25">
+      <c r="K1065" s="19">
         <v>7.79</v>
       </c>
-      <c r="L1065" s="25">
+      <c r="L1065" s="19">
         <v>404.13</v>
       </c>
-      <c r="M1065" s="25" t="s">
+      <c r="M1065" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="N1065" s="31"/>
-      <c r="O1065" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1065" s="25"/>
-      <c r="Q1065" s="25"/>
-      <c r="R1065" s="25"/>
+      <c r="N1065" s="19"/>
+      <c r="O1065" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1065" s="19"/>
+      <c r="Q1065" s="19"/>
+      <c r="R1065" s="19"/>
     </row>
     <row r="1066" spans="1:18">
-      <c r="A1066" s="26">
-        <v>45447</v>
-      </c>
-      <c r="B1066" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1066" s="25" t="s">
+      <c r="A1066" s="20">
+        <v>45447</v>
+      </c>
+      <c r="B1066" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1066" s="19" t="s">
         <v>506</v>
       </c>
-      <c r="D1066" s="25">
-        <v>197402</v>
-      </c>
-      <c r="E1066" s="25">
-        <v>2</v>
-      </c>
-      <c r="F1066" s="27">
+      <c r="D1066" s="19">
+        <v>197402</v>
+      </c>
+      <c r="E1066" s="19">
+        <v>2</v>
+      </c>
+      <c r="F1066" s="21">
         <v>1460607</v>
       </c>
-      <c r="G1066" s="25" t="s">
+      <c r="G1066" s="19" t="s">
         <v>507</v>
       </c>
-      <c r="H1066" s="25" t="s">
+      <c r="H1066" s="19" t="s">
         <v>502</v>
       </c>
-      <c r="I1066" s="28">
+      <c r="I1066" s="22">
         <v>1603783</v>
       </c>
-      <c r="J1066" s="25">
+      <c r="J1066" s="19">
         <v>15</v>
       </c>
-      <c r="K1066" s="25">
+      <c r="K1066" s="19">
         <v>21.7</v>
       </c>
-      <c r="L1066" s="25">
+      <c r="L1066" s="19">
         <v>953.28</v>
       </c>
-      <c r="M1066" s="25" t="s">
+      <c r="M1066" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="N1066" s="31"/>
-      <c r="O1066" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1066" s="25"/>
-      <c r="Q1066" s="25"/>
-      <c r="R1066" s="25"/>
+      <c r="N1066" s="19"/>
+      <c r="O1066" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1066" s="19"/>
+      <c r="Q1066" s="19"/>
+      <c r="R1066" s="19"/>
     </row>
     <row r="1067" spans="1:18">
-      <c r="A1067" s="26">
-        <v>45447</v>
-      </c>
-      <c r="B1067" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1067" s="25" t="s">
+      <c r="A1067" s="20">
+        <v>45447</v>
+      </c>
+      <c r="B1067" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1067" s="19" t="s">
         <v>506</v>
       </c>
-      <c r="D1067" s="25">
-        <v>197402</v>
-      </c>
-      <c r="E1067" s="25">
-        <v>2</v>
-      </c>
-      <c r="F1067" s="27">
+      <c r="D1067" s="19">
+        <v>197402</v>
+      </c>
+      <c r="E1067" s="19">
+        <v>2</v>
+      </c>
+      <c r="F1067" s="21">
         <v>1460608</v>
       </c>
-      <c r="G1067" s="25" t="s">
+      <c r="G1067" s="19" t="s">
         <v>507</v>
       </c>
-      <c r="H1067" s="25" t="s">
+      <c r="H1067" s="19" t="s">
         <v>502</v>
       </c>
-      <c r="I1067" s="28">
+      <c r="I1067" s="22">
         <v>1603783</v>
       </c>
-      <c r="J1067" s="25">
+      <c r="J1067" s="19">
         <v>4</v>
       </c>
-      <c r="K1067" s="25">
+      <c r="K1067" s="19">
         <v>17.920000000000002</v>
       </c>
-      <c r="L1067" s="30">
+      <c r="L1067" s="24">
         <v>1251.72</v>
       </c>
-      <c r="M1067" s="25" t="s">
+      <c r="M1067" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="N1067" s="31"/>
-      <c r="O1067" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1067" s="25"/>
-      <c r="Q1067" s="25"/>
-      <c r="R1067" s="25"/>
+      <c r="N1067" s="19"/>
+      <c r="O1067" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1067" s="19"/>
+      <c r="Q1067" s="19"/>
+      <c r="R1067" s="19"/>
     </row>
     <row r="1068" spans="1:18">
-      <c r="A1068" s="26">
-        <v>45447</v>
-      </c>
-      <c r="B1068" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1068" s="25" t="s">
+      <c r="A1068" s="20">
+        <v>45447</v>
+      </c>
+      <c r="B1068" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1068" s="19" t="s">
         <v>506</v>
       </c>
-      <c r="D1068" s="25">
-        <v>197402</v>
-      </c>
-      <c r="E1068" s="25">
-        <v>2</v>
-      </c>
-      <c r="F1068" s="27">
+      <c r="D1068" s="19">
+        <v>197402</v>
+      </c>
+      <c r="E1068" s="19">
+        <v>2</v>
+      </c>
+      <c r="F1068" s="21">
         <v>1460609</v>
       </c>
-      <c r="G1068" s="25" t="s">
+      <c r="G1068" s="19" t="s">
         <v>507</v>
       </c>
-      <c r="H1068" s="25" t="s">
+      <c r="H1068" s="19" t="s">
         <v>502</v>
       </c>
-      <c r="I1068" s="28">
+      <c r="I1068" s="22">
         <v>1603783</v>
       </c>
-      <c r="J1068" s="25">
+      <c r="J1068" s="19">
         <v>3</v>
       </c>
-      <c r="K1068" s="25">
+      <c r="K1068" s="19">
         <v>7.79</v>
       </c>
-      <c r="L1068" s="25">
+      <c r="L1068" s="19">
         <v>404.13</v>
       </c>
-      <c r="M1068" s="25" t="s">
+      <c r="M1068" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="N1068" s="31"/>
-      <c r="O1068" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1068" s="25"/>
-      <c r="Q1068" s="25"/>
-      <c r="R1068" s="25"/>
+      <c r="N1068" s="19"/>
+      <c r="O1068" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1068" s="19"/>
+      <c r="Q1068" s="19"/>
+      <c r="R1068" s="19"/>
     </row>
     <row r="1069" spans="1:18">
-      <c r="A1069" s="26">
-        <v>45447</v>
-      </c>
-      <c r="B1069" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1069" s="25" t="s">
+      <c r="A1069" s="20">
+        <v>45447</v>
+      </c>
+      <c r="B1069" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1069" s="19" t="s">
         <v>508</v>
       </c>
-      <c r="D1069" s="25">
-        <v>197402</v>
-      </c>
-      <c r="E1069" s="25">
-        <v>2</v>
-      </c>
-      <c r="F1069" s="27">
+      <c r="D1069" s="19">
+        <v>197402</v>
+      </c>
+      <c r="E1069" s="19">
+        <v>2</v>
+      </c>
+      <c r="F1069" s="21">
         <v>1460690</v>
       </c>
-      <c r="G1069" s="25" t="s">
+      <c r="G1069" s="19" t="s">
         <v>509</v>
       </c>
-      <c r="H1069" s="25" t="s">
+      <c r="H1069" s="19" t="s">
         <v>502</v>
       </c>
-      <c r="I1069" s="28">
+      <c r="I1069" s="22">
         <v>1603890</v>
       </c>
-      <c r="J1069" s="25">
+      <c r="J1069" s="19">
         <v>12</v>
       </c>
-      <c r="K1069" s="25">
+      <c r="K1069" s="19">
         <v>16.79</v>
       </c>
-      <c r="L1069" s="25">
+      <c r="L1069" s="19">
         <v>762.63</v>
       </c>
-      <c r="M1069" s="25" t="s">
+      <c r="M1069" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="N1069" s="31"/>
-      <c r="O1069" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1069" s="25"/>
-      <c r="Q1069" s="25"/>
-      <c r="R1069" s="25"/>
+      <c r="N1069" s="19"/>
+      <c r="O1069" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1069" s="19"/>
+      <c r="Q1069" s="19"/>
+      <c r="R1069" s="19"/>
     </row>
     <row r="1070" spans="1:18">
-      <c r="A1070" s="26">
-        <v>45447</v>
-      </c>
-      <c r="B1070" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1070" s="25" t="s">
+      <c r="A1070" s="20">
+        <v>45447</v>
+      </c>
+      <c r="B1070" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1070" s="19" t="s">
         <v>508</v>
       </c>
-      <c r="D1070" s="25">
-        <v>197402</v>
-      </c>
-      <c r="E1070" s="25">
-        <v>2</v>
-      </c>
-      <c r="F1070" s="27">
+      <c r="D1070" s="19">
+        <v>197402</v>
+      </c>
+      <c r="E1070" s="19">
+        <v>2</v>
+      </c>
+      <c r="F1070" s="21">
         <v>1460691</v>
       </c>
-      <c r="G1070" s="25" t="s">
+      <c r="G1070" s="19" t="s">
         <v>509</v>
       </c>
-      <c r="H1070" s="25" t="s">
+      <c r="H1070" s="19" t="s">
         <v>502</v>
       </c>
-      <c r="I1070" s="28">
+      <c r="I1070" s="22">
         <v>1603890</v>
       </c>
-      <c r="J1070" s="25">
+      <c r="J1070" s="19">
         <v>1</v>
       </c>
-      <c r="K1070" s="25">
-        <v>2</v>
-      </c>
-      <c r="L1070" s="25">
+      <c r="K1070" s="19">
+        <v>2</v>
+      </c>
+      <c r="L1070" s="19">
         <v>94.62</v>
       </c>
-      <c r="M1070" s="25" t="s">
+      <c r="M1070" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="N1070" s="31"/>
-      <c r="O1070" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1070" s="25"/>
-      <c r="Q1070" s="25"/>
-      <c r="R1070" s="25"/>
+      <c r="N1070" s="19"/>
+      <c r="O1070" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1070" s="19"/>
+      <c r="Q1070" s="19"/>
+      <c r="R1070" s="19"/>
     </row>
     <row r="1071" spans="1:18">
-      <c r="A1071" s="26">
-        <v>45447</v>
-      </c>
-      <c r="B1071" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1071" s="25" t="s">
+      <c r="A1071" s="20">
+        <v>45447</v>
+      </c>
+      <c r="B1071" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1071" s="19" t="s">
         <v>508</v>
       </c>
-      <c r="D1071" s="25">
-        <v>197402</v>
-      </c>
-      <c r="E1071" s="25">
-        <v>2</v>
-      </c>
-      <c r="F1071" s="27">
+      <c r="D1071" s="19">
+        <v>197402</v>
+      </c>
+      <c r="E1071" s="19">
+        <v>2</v>
+      </c>
+      <c r="F1071" s="21">
         <v>1460692</v>
       </c>
-      <c r="G1071" s="25" t="s">
+      <c r="G1071" s="19" t="s">
         <v>509</v>
       </c>
-      <c r="H1071" s="25" t="s">
+      <c r="H1071" s="19" t="s">
         <v>502</v>
       </c>
-      <c r="I1071" s="28">
+      <c r="I1071" s="22">
         <v>1603890</v>
       </c>
-      <c r="J1071" s="25">
+      <c r="J1071" s="19">
         <v>1</v>
       </c>
-      <c r="K1071" s="25">
+      <c r="K1071" s="19">
         <v>2.37</v>
       </c>
-      <c r="L1071" s="25">
+      <c r="L1071" s="19">
         <v>143.47999999999999</v>
       </c>
-      <c r="M1071" s="25" t="s">
+      <c r="M1071" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="N1071" s="31"/>
-      <c r="O1071" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1071" s="25"/>
-      <c r="Q1071" s="25"/>
-      <c r="R1071" s="25"/>
+      <c r="N1071" s="19"/>
+      <c r="O1071" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1071" s="19"/>
+      <c r="Q1071" s="19"/>
+      <c r="R1071" s="19"/>
     </row>
     <row r="1072" spans="1:18">
-      <c r="A1072" s="26">
-        <v>45447</v>
-      </c>
-      <c r="B1072" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1072" s="25" t="s">
+      <c r="A1072" s="20">
+        <v>45447</v>
+      </c>
+      <c r="B1072" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1072" s="19" t="s">
         <v>508</v>
       </c>
-      <c r="D1072" s="25">
-        <v>197402</v>
-      </c>
-      <c r="E1072" s="25">
-        <v>2</v>
-      </c>
-      <c r="F1072" s="27">
+      <c r="D1072" s="19">
+        <v>197402</v>
+      </c>
+      <c r="E1072" s="19">
+        <v>2</v>
+      </c>
+      <c r="F1072" s="21">
         <v>1460693</v>
       </c>
-      <c r="G1072" s="25" t="s">
+      <c r="G1072" s="19" t="s">
         <v>509</v>
       </c>
-      <c r="H1072" s="25" t="s">
+      <c r="H1072" s="19" t="s">
         <v>502</v>
       </c>
-      <c r="I1072" s="28">
+      <c r="I1072" s="22">
         <v>1603890</v>
       </c>
-      <c r="J1072" s="25">
+      <c r="J1072" s="19">
         <v>3</v>
       </c>
-      <c r="K1072" s="25">
+      <c r="K1072" s="19">
         <v>7.79</v>
       </c>
-      <c r="L1072" s="25">
+      <c r="L1072" s="19">
         <v>404.13</v>
       </c>
-      <c r="M1072" s="25" t="s">
+      <c r="M1072" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="N1072" s="31"/>
-      <c r="O1072" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1072" s="25"/>
-      <c r="Q1072" s="25"/>
-      <c r="R1072" s="25"/>
+      <c r="N1072" s="19"/>
+      <c r="O1072" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1072" s="19"/>
+      <c r="Q1072" s="19"/>
+      <c r="R1072" s="19"/>
+    </row>
+    <row r="1073" spans="1:18">
+      <c r="A1073" s="26">
+        <v>45447</v>
+      </c>
+      <c r="B1073" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1073" s="25" t="s">
+        <v>510</v>
+      </c>
+      <c r="D1073" s="25">
+        <v>197402</v>
+      </c>
+      <c r="E1073" s="25">
+        <v>2</v>
+      </c>
+      <c r="F1073" s="27">
+        <v>1460872</v>
+      </c>
+      <c r="G1073" s="25" t="s">
+        <v>511</v>
+      </c>
+      <c r="H1073" s="25" t="s">
+        <v>502</v>
+      </c>
+      <c r="I1073" s="28">
+        <v>1603885</v>
+      </c>
+      <c r="J1073" s="25">
+        <v>8</v>
+      </c>
+      <c r="K1073" s="25">
+        <v>11.51</v>
+      </c>
+      <c r="L1073" s="25">
+        <v>508.43</v>
+      </c>
+      <c r="M1073" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1073" s="29"/>
+      <c r="O1073" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1073" s="25"/>
+      <c r="Q1073" s="25"/>
+      <c r="R1073" s="25"/>
+    </row>
+    <row r="1074" spans="1:18">
+      <c r="A1074" s="26">
+        <v>45447</v>
+      </c>
+      <c r="B1074" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1074" s="25" t="s">
+        <v>510</v>
+      </c>
+      <c r="D1074" s="25">
+        <v>197402</v>
+      </c>
+      <c r="E1074" s="25">
+        <v>2</v>
+      </c>
+      <c r="F1074" s="27">
+        <v>1460873</v>
+      </c>
+      <c r="G1074" s="25" t="s">
+        <v>511</v>
+      </c>
+      <c r="H1074" s="25" t="s">
+        <v>502</v>
+      </c>
+      <c r="I1074" s="28">
+        <v>1603885</v>
+      </c>
+      <c r="J1074" s="25">
+        <v>1</v>
+      </c>
+      <c r="K1074" s="25">
+        <v>2</v>
+      </c>
+      <c r="L1074" s="25">
+        <v>94.62</v>
+      </c>
+      <c r="M1074" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1074" s="29"/>
+      <c r="O1074" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1074" s="25"/>
+      <c r="Q1074" s="25"/>
+      <c r="R1074" s="25"/>
+    </row>
+    <row r="1075" spans="1:18">
+      <c r="A1075" s="26">
+        <v>45447</v>
+      </c>
+      <c r="B1075" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1075" s="25" t="s">
+        <v>510</v>
+      </c>
+      <c r="D1075" s="25">
+        <v>197402</v>
+      </c>
+      <c r="E1075" s="25">
+        <v>2</v>
+      </c>
+      <c r="F1075" s="27">
+        <v>1460874</v>
+      </c>
+      <c r="G1075" s="25" t="s">
+        <v>511</v>
+      </c>
+      <c r="H1075" s="25" t="s">
+        <v>502</v>
+      </c>
+      <c r="I1075" s="28">
+        <v>1603885</v>
+      </c>
+      <c r="J1075" s="25">
+        <v>1</v>
+      </c>
+      <c r="K1075" s="25">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="L1075" s="25">
+        <v>154.96</v>
+      </c>
+      <c r="M1075" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1075" s="29"/>
+      <c r="O1075" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1075" s="25"/>
+      <c r="Q1075" s="25"/>
+      <c r="R1075" s="25"/>
+    </row>
+    <row r="1076" spans="1:18">
+      <c r="A1076" s="26">
+        <v>45447</v>
+      </c>
+      <c r="B1076" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1076" s="25" t="s">
+        <v>510</v>
+      </c>
+      <c r="D1076" s="25">
+        <v>197402</v>
+      </c>
+      <c r="E1076" s="25">
+        <v>2</v>
+      </c>
+      <c r="F1076" s="27">
+        <v>1460875</v>
+      </c>
+      <c r="G1076" s="25" t="s">
+        <v>511</v>
+      </c>
+      <c r="H1076" s="25" t="s">
+        <v>502</v>
+      </c>
+      <c r="I1076" s="28">
+        <v>1603885</v>
+      </c>
+      <c r="J1076" s="25">
+        <v>1</v>
+      </c>
+      <c r="K1076" s="25">
+        <v>2.97</v>
+      </c>
+      <c r="L1076" s="25">
+        <v>157.28</v>
+      </c>
+      <c r="M1076" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1076" s="29"/>
+      <c r="O1076" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1076" s="25"/>
+      <c r="Q1076" s="25"/>
+      <c r="R1076" s="25"/>
+    </row>
+    <row r="1077" spans="1:18">
+      <c r="A1077" s="26">
+        <v>45447</v>
+      </c>
+      <c r="B1077" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1077" s="25" t="s">
+        <v>512</v>
+      </c>
+      <c r="D1077" s="25">
+        <v>197402</v>
+      </c>
+      <c r="E1077" s="25">
+        <v>2</v>
+      </c>
+      <c r="F1077" s="27">
+        <v>1461016</v>
+      </c>
+      <c r="G1077" s="25" t="s">
+        <v>513</v>
+      </c>
+      <c r="H1077" s="25" t="s">
+        <v>502</v>
+      </c>
+      <c r="I1077" s="28">
+        <v>1603989</v>
+      </c>
+      <c r="J1077" s="25">
+        <v>6</v>
+      </c>
+      <c r="K1077" s="25">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="L1077" s="25">
+        <v>381.32</v>
+      </c>
+      <c r="M1077" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1077" s="29"/>
+      <c r="O1077" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1077" s="25"/>
+      <c r="Q1077" s="25"/>
+      <c r="R1077" s="25"/>
+    </row>
+    <row r="1078" spans="1:18">
+      <c r="A1078" s="26">
+        <v>45447</v>
+      </c>
+      <c r="B1078" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1078" s="25" t="s">
+        <v>512</v>
+      </c>
+      <c r="D1078" s="25">
+        <v>197402</v>
+      </c>
+      <c r="E1078" s="25">
+        <v>2</v>
+      </c>
+      <c r="F1078" s="27">
+        <v>1461017</v>
+      </c>
+      <c r="G1078" s="25" t="s">
+        <v>513</v>
+      </c>
+      <c r="H1078" s="25" t="s">
+        <v>502</v>
+      </c>
+      <c r="I1078" s="28">
+        <v>1603989</v>
+      </c>
+      <c r="J1078" s="25">
+        <v>3</v>
+      </c>
+      <c r="K1078" s="25">
+        <v>5.69</v>
+      </c>
+      <c r="L1078" s="25">
+        <v>268.47000000000003</v>
+      </c>
+      <c r="M1078" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1078" s="29"/>
+      <c r="O1078" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1078" s="25"/>
+      <c r="Q1078" s="25"/>
+      <c r="R1078" s="25"/>
+    </row>
+    <row r="1079" spans="1:18">
+      <c r="A1079" s="26">
+        <v>45447</v>
+      </c>
+      <c r="B1079" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1079" s="25" t="s">
+        <v>512</v>
+      </c>
+      <c r="D1079" s="25">
+        <v>197402</v>
+      </c>
+      <c r="E1079" s="25">
+        <v>2</v>
+      </c>
+      <c r="F1079" s="27">
+        <v>1461018</v>
+      </c>
+      <c r="G1079" s="25" t="s">
+        <v>513</v>
+      </c>
+      <c r="H1079" s="25" t="s">
+        <v>502</v>
+      </c>
+      <c r="I1079" s="28">
+        <v>1603989</v>
+      </c>
+      <c r="J1079" s="25">
+        <v>1</v>
+      </c>
+      <c r="K1079" s="25">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="L1079" s="25">
+        <v>154.96</v>
+      </c>
+      <c r="M1079" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1079" s="29"/>
+      <c r="O1079" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1079" s="25"/>
+      <c r="Q1079" s="25"/>
+      <c r="R1079" s="25"/>
+    </row>
+    <row r="1080" spans="1:18">
+      <c r="A1080" s="26">
+        <v>45447</v>
+      </c>
+      <c r="B1080" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1080" s="25" t="s">
+        <v>512</v>
+      </c>
+      <c r="D1080" s="25">
+        <v>197402</v>
+      </c>
+      <c r="E1080" s="25">
+        <v>2</v>
+      </c>
+      <c r="F1080" s="27">
+        <v>1461019</v>
+      </c>
+      <c r="G1080" s="25" t="s">
+        <v>513</v>
+      </c>
+      <c r="H1080" s="25" t="s">
+        <v>502</v>
+      </c>
+      <c r="I1080" s="28">
+        <v>1603989</v>
+      </c>
+      <c r="J1080" s="25">
+        <v>1</v>
+      </c>
+      <c r="K1080" s="25">
+        <v>2.97</v>
+      </c>
+      <c r="L1080" s="25">
+        <v>157.28</v>
+      </c>
+      <c r="M1080" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1080" s="29"/>
+      <c r="O1080" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1080" s="25"/>
+      <c r="Q1080" s="25"/>
+      <c r="R1080" s="25"/>
+    </row>
+    <row r="1081" spans="1:18">
+      <c r="A1081" s="26">
+        <v>45447</v>
+      </c>
+      <c r="B1081" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1081" s="25" t="s">
+        <v>514</v>
+      </c>
+      <c r="D1081" s="25">
+        <v>197402</v>
+      </c>
+      <c r="E1081" s="25">
+        <v>2</v>
+      </c>
+      <c r="F1081" s="27">
+        <v>1461065</v>
+      </c>
+      <c r="G1081" s="25" t="s">
+        <v>515</v>
+      </c>
+      <c r="H1081" s="25" t="s">
+        <v>502</v>
+      </c>
+      <c r="I1081" s="28">
+        <v>1603780</v>
+      </c>
+      <c r="J1081" s="25">
+        <v>9</v>
+      </c>
+      <c r="K1081" s="25">
+        <v>13.07</v>
+      </c>
+      <c r="L1081" s="25">
+        <v>571.98</v>
+      </c>
+      <c r="M1081" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1081" s="29"/>
+      <c r="O1081" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1081" s="25"/>
+      <c r="Q1081" s="25"/>
+      <c r="R1081" s="25"/>
+    </row>
+    <row r="1082" spans="1:18">
+      <c r="A1082" s="26">
+        <v>45447</v>
+      </c>
+      <c r="B1082" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1082" s="25" t="s">
+        <v>514</v>
+      </c>
+      <c r="D1082" s="25">
+        <v>197402</v>
+      </c>
+      <c r="E1082" s="25">
+        <v>2</v>
+      </c>
+      <c r="F1082" s="27">
+        <v>1461066</v>
+      </c>
+      <c r="G1082" s="25" t="s">
+        <v>515</v>
+      </c>
+      <c r="H1082" s="25" t="s">
+        <v>502</v>
+      </c>
+      <c r="I1082" s="28">
+        <v>1603780</v>
+      </c>
+      <c r="J1082" s="25">
+        <v>6</v>
+      </c>
+      <c r="K1082" s="25">
+        <v>22.7</v>
+      </c>
+      <c r="L1082" s="31">
+        <v>1563.07</v>
+      </c>
+      <c r="M1082" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1082" s="29"/>
+      <c r="O1082" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1082" s="25"/>
+      <c r="Q1082" s="25"/>
+      <c r="R1082" s="25"/>
+    </row>
+    <row r="1083" spans="1:18">
+      <c r="A1083" s="26">
+        <v>45447</v>
+      </c>
+      <c r="B1083" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1083" s="25" t="s">
+        <v>514</v>
+      </c>
+      <c r="D1083" s="25">
+        <v>197402</v>
+      </c>
+      <c r="E1083" s="25">
+        <v>2</v>
+      </c>
+      <c r="F1083" s="27">
+        <v>1461067</v>
+      </c>
+      <c r="G1083" s="25" t="s">
+        <v>515</v>
+      </c>
+      <c r="H1083" s="25" t="s">
+        <v>502</v>
+      </c>
+      <c r="I1083" s="28">
+        <v>1603780</v>
+      </c>
+      <c r="J1083" s="25">
+        <v>1</v>
+      </c>
+      <c r="K1083" s="25">
+        <v>2</v>
+      </c>
+      <c r="L1083" s="25">
+        <v>94.62</v>
+      </c>
+      <c r="M1083" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1083" s="29"/>
+      <c r="O1083" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1083" s="25"/>
+      <c r="Q1083" s="25"/>
+      <c r="R1083" s="25"/>
+    </row>
+    <row r="1084" spans="1:18">
+      <c r="A1084" s="26">
+        <v>45447</v>
+      </c>
+      <c r="B1084" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1084" s="25" t="s">
+        <v>514</v>
+      </c>
+      <c r="D1084" s="25">
+        <v>197402</v>
+      </c>
+      <c r="E1084" s="25">
+        <v>2</v>
+      </c>
+      <c r="F1084" s="27">
+        <v>1461068</v>
+      </c>
+      <c r="G1084" s="25" t="s">
+        <v>515</v>
+      </c>
+      <c r="H1084" s="25" t="s">
+        <v>502</v>
+      </c>
+      <c r="I1084" s="28">
+        <v>1603780</v>
+      </c>
+      <c r="J1084" s="25">
+        <v>1</v>
+      </c>
+      <c r="K1084" s="25">
+        <v>2.97</v>
+      </c>
+      <c r="L1084" s="25">
+        <v>157.28</v>
+      </c>
+      <c r="M1084" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1084" s="29"/>
+      <c r="O1084" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1084" s="25"/>
+      <c r="Q1084" s="25"/>
+      <c r="R1084" s="25"/>
+    </row>
+    <row r="1085" spans="1:18">
+      <c r="A1085" s="26">
+        <v>45447</v>
+      </c>
+      <c r="B1085" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1085" s="25" t="s">
+        <v>516</v>
+      </c>
+      <c r="D1085" s="25">
+        <v>197402</v>
+      </c>
+      <c r="E1085" s="25">
+        <v>2</v>
+      </c>
+      <c r="F1085" s="27">
+        <v>1461106</v>
+      </c>
+      <c r="G1085" s="25" t="s">
+        <v>517</v>
+      </c>
+      <c r="H1085" s="25" t="s">
+        <v>502</v>
+      </c>
+      <c r="I1085" s="28">
+        <v>1603757</v>
+      </c>
+      <c r="J1085" s="25">
+        <v>28</v>
+      </c>
+      <c r="K1085" s="25">
+        <v>40.04</v>
+      </c>
+      <c r="L1085" s="31">
+        <v>1779.45</v>
+      </c>
+      <c r="M1085" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1085" s="29"/>
+      <c r="O1085" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1085" s="25"/>
+      <c r="Q1085" s="25"/>
+      <c r="R1085" s="25"/>
+    </row>
+    <row r="1086" spans="1:18">
+      <c r="A1086" s="26">
+        <v>45447</v>
+      </c>
+      <c r="B1086" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1086" s="25" t="s">
+        <v>516</v>
+      </c>
+      <c r="D1086" s="25">
+        <v>197402</v>
+      </c>
+      <c r="E1086" s="25">
+        <v>2</v>
+      </c>
+      <c r="F1086" s="27">
+        <v>1461107</v>
+      </c>
+      <c r="G1086" s="25" t="s">
+        <v>517</v>
+      </c>
+      <c r="H1086" s="25" t="s">
+        <v>502</v>
+      </c>
+      <c r="I1086" s="28">
+        <v>1603757</v>
+      </c>
+      <c r="J1086" s="25">
+        <v>9</v>
+      </c>
+      <c r="K1086" s="25">
+        <v>40.32</v>
+      </c>
+      <c r="L1086" s="31">
+        <v>2816.39</v>
+      </c>
+      <c r="M1086" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1086" s="29"/>
+      <c r="O1086" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1086" s="25"/>
+      <c r="Q1086" s="25"/>
+      <c r="R1086" s="25"/>
+    </row>
+    <row r="1087" spans="1:18">
+      <c r="A1087" s="26">
+        <v>45447</v>
+      </c>
+      <c r="B1087" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1087" s="25" t="s">
+        <v>516</v>
+      </c>
+      <c r="D1087" s="25">
+        <v>197402</v>
+      </c>
+      <c r="E1087" s="25">
+        <v>2</v>
+      </c>
+      <c r="F1087" s="27">
+        <v>1461108</v>
+      </c>
+      <c r="G1087" s="25" t="s">
+        <v>517</v>
+      </c>
+      <c r="H1087" s="25" t="s">
+        <v>502</v>
+      </c>
+      <c r="I1087" s="28">
+        <v>1603757</v>
+      </c>
+      <c r="J1087" s="25">
+        <v>3</v>
+      </c>
+      <c r="K1087" s="25">
+        <v>6</v>
+      </c>
+      <c r="L1087" s="25">
+        <v>283.86</v>
+      </c>
+      <c r="M1087" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1087" s="29"/>
+      <c r="O1087" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1087" s="25"/>
+      <c r="Q1087" s="25"/>
+      <c r="R1087" s="25"/>
+    </row>
+    <row r="1088" spans="1:18">
+      <c r="A1088" s="26">
+        <v>45447</v>
+      </c>
+      <c r="B1088" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1088" s="25" t="s">
+        <v>516</v>
+      </c>
+      <c r="D1088" s="25">
+        <v>197402</v>
+      </c>
+      <c r="E1088" s="25">
+        <v>2</v>
+      </c>
+      <c r="F1088" s="27">
+        <v>1461109</v>
+      </c>
+      <c r="G1088" s="25" t="s">
+        <v>517</v>
+      </c>
+      <c r="H1088" s="25" t="s">
+        <v>502</v>
+      </c>
+      <c r="I1088" s="28">
+        <v>1603757</v>
+      </c>
+      <c r="J1088" s="25">
+        <v>9</v>
+      </c>
+      <c r="K1088" s="25">
+        <v>22.23</v>
+      </c>
+      <c r="L1088" s="31">
+        <v>1144.73</v>
+      </c>
+      <c r="M1088" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1088" s="29"/>
+      <c r="O1088" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1088" s="25"/>
+      <c r="Q1088" s="25"/>
+      <c r="R1088" s="25"/>
+    </row>
+    <row r="1089" spans="1:18">
+      <c r="A1089" s="26">
+        <v>45447</v>
+      </c>
+      <c r="B1089" s="25" t="s">
+        <v>326</v>
+      </c>
+      <c r="C1089" s="25" t="s">
+        <v>510</v>
+      </c>
+      <c r="D1089" s="25">
+        <v>197570</v>
+      </c>
+      <c r="E1089" s="25">
+        <v>2</v>
+      </c>
+      <c r="F1089" s="27">
+        <v>1469093</v>
+      </c>
+      <c r="G1089" s="25" t="s">
+        <v>511</v>
+      </c>
+      <c r="H1089" s="25" t="s">
+        <v>502</v>
+      </c>
+      <c r="I1089" s="28">
+        <v>1605471</v>
+      </c>
+      <c r="J1089" s="25">
+        <v>5</v>
+      </c>
+      <c r="K1089" s="25">
+        <v>9.3699999999999992</v>
+      </c>
+      <c r="L1089" s="25">
+        <v>630.91999999999996</v>
+      </c>
+      <c r="M1089" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1089" s="29"/>
+      <c r="O1089" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1089" s="25"/>
+      <c r="Q1089" s="25"/>
+      <c r="R1089" s="25"/>
+    </row>
+    <row r="1090" spans="1:18">
+      <c r="A1090" s="26">
+        <v>45447</v>
+      </c>
+      <c r="B1090" s="25" t="s">
+        <v>326</v>
+      </c>
+      <c r="C1090" s="25" t="s">
+        <v>510</v>
+      </c>
+      <c r="D1090" s="25">
+        <v>197570</v>
+      </c>
+      <c r="E1090" s="25">
+        <v>2</v>
+      </c>
+      <c r="F1090" s="27">
+        <v>1469094</v>
+      </c>
+      <c r="G1090" s="25" t="s">
+        <v>511</v>
+      </c>
+      <c r="H1090" s="25" t="s">
+        <v>502</v>
+      </c>
+      <c r="I1090" s="28">
+        <v>1605471</v>
+      </c>
+      <c r="J1090" s="25">
+        <v>1</v>
+      </c>
+      <c r="K1090" s="25">
+        <v>2.25</v>
+      </c>
+      <c r="L1090" s="25">
+        <v>208.31</v>
+      </c>
+      <c r="M1090" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1090" s="29"/>
+      <c r="O1090" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1090" s="25"/>
+      <c r="Q1090" s="25"/>
+      <c r="R1090" s="25"/>
+    </row>
+    <row r="1091" spans="1:18">
+      <c r="A1091" s="26">
+        <v>45447</v>
+      </c>
+      <c r="B1091" s="25" t="s">
+        <v>326</v>
+      </c>
+      <c r="C1091" s="25" t="s">
+        <v>512</v>
+      </c>
+      <c r="D1091" s="25">
+        <v>197570</v>
+      </c>
+      <c r="E1091" s="25">
+        <v>2</v>
+      </c>
+      <c r="F1091" s="27">
+        <v>1469199</v>
+      </c>
+      <c r="G1091" s="25" t="s">
+        <v>513</v>
+      </c>
+      <c r="H1091" s="25" t="s">
+        <v>502</v>
+      </c>
+      <c r="I1091" s="28">
+        <v>1605576</v>
+      </c>
+      <c r="J1091" s="25">
+        <v>3</v>
+      </c>
+      <c r="K1091" s="25">
+        <v>5.61</v>
+      </c>
+      <c r="L1091" s="25">
+        <v>501.79</v>
+      </c>
+      <c r="M1091" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1091" s="29"/>
+      <c r="O1091" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1091" s="25"/>
+      <c r="Q1091" s="25"/>
+      <c r="R1091" s="25"/>
+    </row>
+    <row r="1092" spans="1:18">
+      <c r="A1092" s="26">
+        <v>45447</v>
+      </c>
+      <c r="B1092" s="25" t="s">
+        <v>326</v>
+      </c>
+      <c r="C1092" s="25" t="s">
+        <v>512</v>
+      </c>
+      <c r="D1092" s="25">
+        <v>197570</v>
+      </c>
+      <c r="E1092" s="25">
+        <v>2</v>
+      </c>
+      <c r="F1092" s="27">
+        <v>1469200</v>
+      </c>
+      <c r="G1092" s="25" t="s">
+        <v>513</v>
+      </c>
+      <c r="H1092" s="25" t="s">
+        <v>502</v>
+      </c>
+      <c r="I1092" s="28">
+        <v>1605576</v>
+      </c>
+      <c r="J1092" s="25">
+        <v>6</v>
+      </c>
+      <c r="K1092" s="25">
+        <v>18.3</v>
+      </c>
+      <c r="L1092" s="31">
+        <v>1167.74</v>
+      </c>
+      <c r="M1092" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1092" s="29"/>
+      <c r="O1092" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1092" s="25"/>
+      <c r="Q1092" s="25"/>
+      <c r="R1092" s="25"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="O2:O29 O31:O79 O81:O204">

</xml_diff>